<commit_message>
view objects and effectivity satellite
</commit_message>
<xml_diff>
--- a/metadata_ddl/Excel/turbovault4dbt_TPCH.xlsx
+++ b/metadata_ddl/Excel/turbovault4dbt_TPCH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\software\datavaultstarter\turbovault4dbt\metadata_ddl\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e720170\software\datavaultstarter7\turbovault4dbt\metadata_ddl\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDA9C96-85CE-4B3D-9550-277CB88C8D10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C7FB7C-AED0-4B01-B59F-45D0A19220EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="38625" windowHeight="21105" tabRatio="792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="38625" windowHeight="21105" tabRatio="792" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="source_data" sheetId="8" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="standard_satellite" sheetId="3" r:id="rId4"/>
     <sheet name="multiactive_satellite" sheetId="4" r:id="rId5"/>
     <sheet name="non_historized_link" sheetId="5" r:id="rId6"/>
-    <sheet name="non_historized_satellite" sheetId="6" r:id="rId7"/>
-    <sheet name="pit" sheetId="7" r:id="rId8"/>
+    <sheet name="link_eff_satellite" sheetId="9" r:id="rId7"/>
+    <sheet name="non_historized_satellite" sheetId="6" r:id="rId8"/>
+    <sheet name="pit" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="65001"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="125">
   <si>
     <t>Hub_Identifier</t>
   </si>
@@ -396,7 +397,13 @@
     <t>FK_CUST_CUSP</t>
   </si>
   <si>
-    <t>dwhstage</t>
+    <t>cdwh_stg_010138_dynamics</t>
+  </si>
+  <si>
+    <t>Link_Effectivity_Satellite</t>
+  </si>
+  <si>
+    <t>Driving_Key</t>
   </si>
 </sst>
 </file>
@@ -495,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -518,6 +525,18 @@
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -738,8 +757,8 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -912,8 +931,8 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1199,10 +1218,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1228,63 +1247,72 @@
     <col min="20" max="20" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:21" s="18" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="U1" s="17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1310,26 +1338,23 @@
       <c r="L2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>118</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>2</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>102</v>
       </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1354,26 +1379,23 @@
       <c r="L3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>119</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>102</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>96</v>
       </c>
@@ -1395,21 +1417,18 @@
       <c r="L4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1">
+      <c r="N4" s="1"/>
+      <c r="O4" s="1">
         <v>1</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>96</v>
       </c>
@@ -1441,21 +1460,18 @@
       <c r="L5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="M5" s="1"/>
-      <c r="N5">
+      <c r="N5" s="1"/>
+      <c r="O5">
         <v>2</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5" s="5" t="s">
+      <c r="U5" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1468,7 +1484,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1492,11 +1508,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1515,7 +1531,7 @@
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
@@ -1555,8 +1571,9 @@
       <c r="M1" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>64</v>
       </c>
@@ -1594,7 +1611,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
@@ -1632,7 +1649,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
@@ -1664,7 +1681,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
@@ -1702,7 +1719,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
@@ -1740,7 +1757,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -1778,7 +1795,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1789,7 +1806,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1800,7 +1817,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1811,7 +1828,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1822,7 +1839,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1833,7 +1850,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1844,7 +1861,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1855,7 +1872,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1866,7 +1883,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1934,8 +1951,8 @@
     </row>
     <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1953,17 +1970,6 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1978,8 +1984,8 @@
   </sheetPr>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2111,7 +2117,7 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
@@ -2166,10 +2172,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2190,57 +2196,66 @@
     <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:19" s="18" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="P1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="Q1" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="S1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="P1" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="4"/>
       <c r="C2" s="1"/>
@@ -2251,7 +2266,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="1"/>
@@ -2262,27 +2277,27 @@
       <c r="L3" s="1"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
     </row>
   </sheetData>
@@ -2292,6 +2307,45 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2006DB15-0C0B-4C55-92BA-F7D12BC662AC}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2299,7 +2353,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2479,7 +2533,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>